<commit_message>
Extent report fully implemented with overriden assert class
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -80,10 +80,10 @@
     <t>deleteCustomer</t>
   </si>
   <si>
-    <t>cus_H3kv7w75JgdeGy</t>
-  </si>
-  <si>
-    <t>cus_H0So4YQfL0Mv1q</t>
+    <t>cus_H4UfXFvcyIAryp</t>
+  </si>
+  <si>
+    <t>cus_H4Uaiet9m8mye3</t>
   </si>
 </sst>
 </file>
@@ -447,7 +447,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B13" sqref="B13:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
POJO added and create order test created
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="33">
   <si>
     <t>TestData</t>
   </si>
@@ -84,6 +84,36 @@
   </si>
   <si>
     <t>cus_H4Uaiet9m8mye3</t>
+  </si>
+  <si>
+    <t>createPaypalOrder</t>
+  </si>
+  <si>
+    <t>intent</t>
+  </si>
+  <si>
+    <t>currency_code</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>CAPTURE</t>
+  </si>
+  <si>
+    <t>INR</t>
+  </si>
+  <si>
+    <t>getPaypalOrder</t>
+  </si>
+  <si>
+    <t>orderId</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>7YA93243NU2020819</t>
   </si>
 </sst>
 </file>
@@ -444,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:B14"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,6 +607,78 @@
       </c>
       <c r="B14" s="3" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22">
+        <v>500</v>
+      </c>
+      <c r="E22" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Asserions modified, all test cases added
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -7,49 +7,25 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="StripeAPI" sheetId="1" r:id="rId1"/>
+    <sheet name="PaypalAPI" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="28">
   <si>
     <t>TestData</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Id</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
     <t>ABC</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>PQR</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>Method2</t>
-  </si>
-  <si>
-    <t>Ida</t>
-  </si>
-  <si>
     <t>updateCustomer</t>
   </si>
   <si>
@@ -80,12 +56,6 @@
     <t>deleteCustomer</t>
   </si>
   <si>
-    <t>cus_H4UfXFvcyIAryp</t>
-  </si>
-  <si>
-    <t>cus_H4Uaiet9m8mye3</t>
-  </si>
-  <si>
     <t>createPaypalOrder</t>
   </si>
   <si>
@@ -101,9 +71,6 @@
     <t>CAPTURE</t>
   </si>
   <si>
-    <t>INR</t>
-  </si>
-  <si>
     <t>getPaypalOrder</t>
   </si>
   <si>
@@ -113,7 +80,25 @@
     <t>USD</t>
   </si>
   <si>
-    <t>7YA93243NU2020819</t>
+    <t>createPaypalOrderInvalidData</t>
+  </si>
+  <si>
+    <t>CAPTUREss</t>
+  </si>
+  <si>
+    <t>Rupee</t>
+  </si>
+  <si>
+    <t>500.00</t>
+  </si>
+  <si>
+    <t>3TT14747RA4023328</t>
+  </si>
+  <si>
+    <t>cus_H4UXTAj1ED5sCg</t>
+  </si>
+  <si>
+    <t>cus_H4UXAHhIAIICO1</t>
   </si>
 </sst>
 </file>
@@ -166,9 +151,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -474,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,7 +473,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -496,46 +481,46 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>21</v>
+        <v>7</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>16</v>
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>22</v>
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -543,46 +528,46 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>14</v>
+        <v>1</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>21</v>
+        <v>7</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>16</v>
+        <v>1</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>22</v>
+        <v>9</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -590,95 +575,23 @@
         <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>21</v>
+        <v>1</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="C18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21" t="s">
-        <v>26</v>
-      </c>
-      <c r="E21" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22">
-        <v>500</v>
-      </c>
-      <c r="E22" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -695,62 +608,152 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="9.140625" style="3"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="1" t="b">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>